<commit_message>
Adicionado, categorias, graficos, e mais...
</commit_message>
<xml_diff>
--- a/Minhas_Contas.xlsx
+++ b/Minhas_Contas.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,13 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +442,30 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Descricao</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Categoria</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Valor</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Vencimento</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -473,21 +474,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gasolina</t>
+          <t>Entrada</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>46054</v>
+          <t>Sálario</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pagamentos</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>3000</v>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Pago</t>
         </is>

</xml_diff>